<commit_message>
upgrade dha truthing data organization function
</commit_message>
<xml_diff>
--- a/Documents/Log_info.xlsx
+++ b/Documents/Log_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ziweishi/Documents/ziwei_project/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6DB6C8E-ECF6-A546-AF4F-8828BE7BD80B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A82F4A5-BA55-DE4C-B807-740B4812C9B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36460" yWindow="-8520" windowWidth="28040" windowHeight="17340" xr2:uid="{5C42EF7D-A058-0C49-9E2B-148241C5F643}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="38">
   <si>
     <t>site</t>
   </si>
@@ -56,9 +56,6 @@
     <t>nynw</t>
   </si>
   <si>
-    <t>09_19_2023</t>
-  </si>
-  <si>
     <t>whfa</t>
   </si>
   <si>
@@ -68,36 +65,18 @@
     <t>mentoh</t>
   </si>
   <si>
-    <t>09_08_2023</t>
-  </si>
-  <si>
     <t>grovoh</t>
   </si>
   <si>
-    <t>09_07_2023</t>
-  </si>
-  <si>
     <t>lahdfu</t>
   </si>
   <si>
-    <t>08_22_2023</t>
-  </si>
-  <si>
     <t>encinogho</t>
   </si>
   <si>
-    <t>08_18_2023</t>
-  </si>
-  <si>
     <t>hilloh</t>
   </si>
   <si>
-    <t>08_23_2023</t>
-  </si>
-  <si>
-    <t>EQ</t>
-  </si>
-  <si>
     <t>Site_Num</t>
   </si>
   <si>
@@ -128,37 +107,52 @@
     <t>EQ-427</t>
   </si>
   <si>
-    <t>nynw-08_22_2023-EQ-368</t>
-  </si>
-  <si>
-    <t>nynw-09_19_2023-EQ-368</t>
-  </si>
-  <si>
-    <t>ocer-09_07_2023-EQ-363</t>
-  </si>
-  <si>
-    <t>ocer-09_19_2023-EQ-363</t>
-  </si>
-  <si>
-    <t>whfa-08_23_2023-EQ-367</t>
-  </si>
-  <si>
-    <t>whfa-09_19_2023-EQ-67</t>
-  </si>
-  <si>
-    <t>hilloh-08_23_2023-EQ-403</t>
-  </si>
-  <si>
-    <t>grovoh-09_07_2023-EQ-359</t>
-  </si>
-  <si>
-    <t>mentoh-09_08_2023-EQ-421</t>
-  </si>
-  <si>
-    <t>encinogho-08_18_2023-EQ-428</t>
-  </si>
-  <si>
-    <t>lahdfu-08_22_2023-EQ-427</t>
+    <t>08_22_23</t>
+  </si>
+  <si>
+    <t>09_19_23</t>
+  </si>
+  <si>
+    <t>09_07_23</t>
+  </si>
+  <si>
+    <t>08_23_23</t>
+  </si>
+  <si>
+    <t>09_08_23</t>
+  </si>
+  <si>
+    <t>08_18_23</t>
+  </si>
+  <si>
+    <t>EQ_num</t>
+  </si>
+  <si>
+    <t>Northwell</t>
+  </si>
+  <si>
+    <t>Circleville</t>
+  </si>
+  <si>
+    <t>Houston</t>
+  </si>
+  <si>
+    <t>Hilliard</t>
+  </si>
+  <si>
+    <t>Mentor OH</t>
+  </si>
+  <si>
+    <t>Encinogho</t>
+  </si>
+  <si>
+    <t>LA Site</t>
+  </si>
+  <si>
+    <t>Site_Name</t>
+  </si>
+  <si>
+    <t>Grove city</t>
   </si>
 </sst>
 </file>
@@ -530,27 +524,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E91EB16-03FE-924E-AD35-82C0818E88F9}">
-  <dimension ref="B1:G12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="10.83203125" style="2"/>
-    <col min="5" max="5" width="11.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" style="2" customWidth="1"/>
+    <col min="2" max="4" width="10.83203125" style="2"/>
+    <col min="5" max="5" width="11.6640625" style="2" customWidth="1"/>
     <col min="6" max="6" width="10.83203125" style="2"/>
     <col min="7" max="7" width="31.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -559,10 +554,16 @@
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
@@ -573,16 +574,19 @@
         <v>4</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
@@ -593,16 +597,19 @@
         <v>4</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
@@ -610,19 +617,22 @@
         <v>202</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
@@ -630,19 +640,22 @@
         <v>202</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
       <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
@@ -650,19 +663,22 @@
         <v>203</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
@@ -670,19 +686,22 @@
         <v>203</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>3</v>
       </c>
@@ -690,19 +709,22 @@
         <v>207</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="G8" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
       <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
@@ -710,19 +732,22 @@
         <v>208</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
       <c r="B10" s="2" t="s">
         <v>3</v>
       </c>
@@ -730,19 +755,22 @@
         <v>209</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>3</v>
       </c>
@@ -750,19 +778,22 @@
         <v>210</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
       <c r="B12" s="2" t="s">
         <v>3</v>
       </c>
@@ -770,16 +801,16 @@
         <v>211</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>